<commit_message>
Akhil - Frontend Part 1
</commit_message>
<xml_diff>
--- a/XL Spreadsheets/ChallengeMap.xlsx
+++ b/XL Spreadsheets/ChallengeMap.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A0:F1"/>
+  <dimension ref="A0:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,65 +424,157 @@
     <row r="0">
       <c r="A0" t="inlineStr">
         <is>
-          <t>gameID</t>
+          <t>gQ9xLuRH</t>
         </is>
       </c>
       <c r="B0" t="inlineStr">
         <is>
-          <t>challenger</t>
-        </is>
-      </c>
-      <c r="C0" t="inlineStr">
-        <is>
-          <t>rating</t>
-        </is>
-      </c>
-      <c r="D0" t="inlineStr">
-        <is>
-          <t>wager</t>
-        </is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C0" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D0" t="n">
+        <v>100</v>
       </c>
       <c r="E0" t="inlineStr">
         <is>
-          <t>link</t>
-        </is>
-      </c>
-      <c r="F0" t="inlineStr">
-        <is>
-          <t>escrowID</t>
-        </is>
+          <t>https://lichess.org/gQ9xLuRH</t>
+        </is>
+      </c>
+      <c r="F0" t="n">
+        <v>2263</v>
       </c>
     </row>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>gameID</t>
+          <t>kVAJt85j</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>challenger</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>rating</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>wager</t>
-        </is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D1" t="n">
+        <v>100</v>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>link</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>escrowID</t>
-        </is>
+          <t>https://lichess.org/kVAJt85j</t>
+        </is>
+      </c>
+      <c r="F1" t="n">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>W26Ykr8M</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D2" t="n">
+        <v>100</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://lichess.org/W26Ykr8M</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>6ZBZX1lE</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D3" t="n">
+        <v>100</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://lichess.org/6ZBZX1lE</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>T5XjC3ky</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://lichess.org/T5XjC3ky</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1Y81gpYC</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D5" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://lichess.org/1Y81gpYC</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>2315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Accept Button & Stuff
</commit_message>
<xml_diff>
--- a/XL Spreadsheets/ChallengeMap.xlsx
+++ b/XL Spreadsheets/ChallengeMap.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A0:F5"/>
+  <dimension ref="A0:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,7 @@
     <row r="0">
       <c r="A0" t="inlineStr">
         <is>
-          <t>gQ9xLuRH</t>
+          <t>emGkGkKl</t>
         </is>
       </c>
       <c r="B0" t="inlineStr">
@@ -440,43 +440,49 @@
       </c>
       <c r="E0" t="inlineStr">
         <is>
-          <t>https://lichess.org/gQ9xLuRH</t>
+          <t>https://lichess.org/emGkGkKl</t>
         </is>
       </c>
       <c r="F0" t="n">
-        <v>2263</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>kVAJt85j</t>
+          <t>gameID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>trashboatsr</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
-        <v>1818</v>
-      </c>
-      <c r="D1" t="n">
-        <v>100</v>
+          <t>challenger</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>rating</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>wager</t>
+        </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>https://lichess.org/kVAJt85j</t>
-        </is>
-      </c>
-      <c r="F1" t="n">
-        <v>2272</v>
+          <t>link</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>escrowID</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>W26Ykr8M</t>
+          <t>p2LYrWLC</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -492,17 +498,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://lichess.org/W26Ykr8M</t>
+          <t>https://lichess.org/p2LYrWLC</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>2273</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>6ZBZX1lE</t>
+          <t>oIOLTnRN</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -518,17 +524,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://lichess.org/6ZBZX1lE</t>
+          <t>https://lichess.org/oIOLTnRN</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2309</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>T5XjC3ky</t>
+          <t>NHiX7o3n</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -544,17 +550,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://lichess.org/T5XjC3ky</t>
+          <t>https://lichess.org/NHiX7o3n</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2314</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1Y81gpYC</t>
+          <t>YVTmakze</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -570,11 +576,89 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://lichess.org/1Y81gpYC</t>
+          <t>https://lichess.org/YVTmakze</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>2315</v>
+        <v>2562</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>gcDcW4K8</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://lichess.org/gcDcW4K8</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>2564</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>8dQmNTlC</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D7" t="n">
+        <v>100</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://lichess.org/8dQmNTlC</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>532PWje3</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D8" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://lichess.org/532PWje3</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>2566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the fail statuses
</commit_message>
<xml_diff>
--- a/XL Spreadsheets/ChallengeMap.xlsx
+++ b/XL Spreadsheets/ChallengeMap.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A0:F8"/>
+  <dimension ref="A0:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,27 +424,33 @@
     <row r="0">
       <c r="A0" t="inlineStr">
         <is>
-          <t>emGkGkKl</t>
+          <t>gameID</t>
         </is>
       </c>
       <c r="B0" t="inlineStr">
         <is>
-          <t>trashboatsr</t>
-        </is>
-      </c>
-      <c r="C0" t="n">
-        <v>1818</v>
-      </c>
-      <c r="D0" t="n">
-        <v>100</v>
+          <t>challenger</t>
+        </is>
+      </c>
+      <c r="C0" t="inlineStr">
+        <is>
+          <t>rating</t>
+        </is>
+      </c>
+      <c r="D0" t="inlineStr">
+        <is>
+          <t>wager</t>
+        </is>
       </c>
       <c r="E0" t="inlineStr">
         <is>
-          <t>https://lichess.org/emGkGkKl</t>
-        </is>
-      </c>
-      <c r="F0" t="n">
-        <v>2317</v>
+          <t>link</t>
+        </is>
+      </c>
+      <c r="F0" t="inlineStr">
+        <is>
+          <t>escrowID</t>
+        </is>
       </c>
     </row>
     <row r="1">
@@ -478,187 +484,10 @@
           <t>escrowID</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>p2LYrWLC</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>trashboatsr</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1818</v>
-      </c>
-      <c r="D2" t="n">
-        <v>100</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>https://lichess.org/p2LYrWLC</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>2559</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>oIOLTnRN</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>trashboatsr</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1818</v>
-      </c>
-      <c r="D3" t="n">
-        <v>100</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>https://lichess.org/oIOLTnRN</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>2560</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>NHiX7o3n</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>trashboatsr</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1818</v>
-      </c>
-      <c r="D4" t="n">
-        <v>100</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>https://lichess.org/NHiX7o3n</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>2561</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>YVTmakze</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>trashboatsr</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1818</v>
-      </c>
-      <c r="D5" t="n">
-        <v>100</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>https://lichess.org/YVTmakze</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>2562</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>gcDcW4K8</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>trashboatsr</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1818</v>
-      </c>
-      <c r="D6" t="n">
-        <v>100</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>https://lichess.org/gcDcW4K8</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>2564</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>8dQmNTlC</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>trashboatsr</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1818</v>
-      </c>
-      <c r="D7" t="n">
-        <v>100</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>https://lichess.org/8dQmNTlC</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>2565</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>532PWje3</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>trashboatsr</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1818</v>
-      </c>
-      <c r="D8" t="n">
-        <v>100</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>https://lichess.org/532PWje3</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>2566</v>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>accepted?</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'accepter' column & improved rendering on frontend
</commit_message>
<xml_diff>
--- a/XL Spreadsheets/ChallengeMap.xlsx
+++ b/XL Spreadsheets/ChallengeMap.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A0:G1"/>
+  <dimension ref="A0:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,33 +424,30 @@
     <row r="0">
       <c r="A0" t="inlineStr">
         <is>
-          <t>gameID</t>
+          <t>DTZIC6Yj</t>
         </is>
       </c>
       <c r="B0" t="inlineStr">
         <is>
-          <t>challenger</t>
-        </is>
-      </c>
-      <c r="C0" t="inlineStr">
-        <is>
-          <t>rating</t>
-        </is>
-      </c>
-      <c r="D0" t="inlineStr">
-        <is>
-          <t>wager</t>
-        </is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C0" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D0" t="n">
+        <v>200</v>
       </c>
       <c r="E0" t="inlineStr">
         <is>
-          <t>link</t>
-        </is>
-      </c>
-      <c r="F0" t="inlineStr">
-        <is>
-          <t>escrowID</t>
-        </is>
+          <t>https://lichess.org/DTZIC6Yj</t>
+        </is>
+      </c>
+      <c r="F0" t="n">
+        <v>2879</v>
+      </c>
+      <c r="G0" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1">
@@ -487,6 +484,79 @@
       <c r="G1" t="inlineStr">
         <is>
           <t>accepted?</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>accepter</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>O8X0smRx</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D2" t="n">
+        <v>120</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://lichess.org/O8X0smRx</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>2883</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>thorn</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>NAFalFij</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D3" t="n">
+        <v>130</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://lichess.org/NAFalFij</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>2884</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>thorn</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Polished up frontend code
</commit_message>
<xml_diff>
--- a/XL Spreadsheets/ChallengeMap.xlsx
+++ b/XL Spreadsheets/ChallengeMap.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A0:H3"/>
+  <dimension ref="A0:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,6 +560,176 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>7b1DtX5u</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D4" t="n">
+        <v>170</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://lichess.org/7b1DtX5u</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>2886</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>newguy</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GHSOa063</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D5" t="n">
+        <v>140</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://lichess.org/GHSOa063</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>2887</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>BLANK</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>tXRhbtBp</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D6" t="n">
+        <v>180</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://lichess.org/tXRhbtBp</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>2889</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>blank</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>h3KmFj3w</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D7" t="n">
+        <v>210</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://lichess.org/h3KmFj3w</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>2890</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>blank</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>IJQleUwj</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D8" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://lichess.org/IJQleUwj</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>2912</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>blank</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
LichessID included in sign-up
</commit_message>
<xml_diff>
--- a/XL Spreadsheets/ChallengeMap.xlsx
+++ b/XL Spreadsheets/ChallengeMap.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A0:H13"/>
+  <dimension ref="A0:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -900,6 +900,40 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1077ngjy</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D14" t="n">
+        <v>100</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://lichess.org/1077ngjy</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>2992</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>blank</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Everything runs w/ npm start :)
</commit_message>
<xml_diff>
--- a/XL Spreadsheets/ChallengeMap.xlsx
+++ b/XL Spreadsheets/ChallengeMap.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A0:H2"/>
+  <dimension ref="A0:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,6 +526,40 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ABxocmbB</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1818</v>
+      </c>
+      <c r="D3" t="n">
+        <v>100</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://lichess.org/ABxocmbB</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>3024</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>blank</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added currentLichessUser to Frontend
</commit_message>
<xml_diff>
--- a/XL Spreadsheets/ChallengeMap.xlsx
+++ b/XL Spreadsheets/ChallengeMap.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,7 +543,40 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1"/>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>mna6nw74</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1890</v>
+      </c>
+      <c r="D3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://lichess.org/mna6nw74</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>4041</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>blank</t>
+        </is>
+      </c>
+    </row>
     <row r="4" ht="18.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
One Lichess per account
</commit_message>
<xml_diff>
--- a/XL Spreadsheets/ChallengeMap.xlsx
+++ b/XL Spreadsheets/ChallengeMap.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -577,7 +577,40 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="18.75" customHeight="1"/>
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>irBHYEJS</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>trashboatsr</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1890</v>
+      </c>
+      <c r="D4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://lichess.org/irBHYEJS</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>4042</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>blank</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed UI & npm issues
</commit_message>
<xml_diff>
--- a/XL Spreadsheets/ChallengeMap.xlsx
+++ b/XL Spreadsheets/ChallengeMap.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,7 +512,7 @@
     <row r="2" ht="18.75" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Fd2JcWFL</t>
+          <t>bvarNUA0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -528,11 +528,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://lichess.org/Fd2JcWFL</t>
+          <t>https://lichess.org/bvarNUA0</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>4040</v>
+        <v>4087</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -543,74 +543,8 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>mna6nw74</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>trashboatsr</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1890</v>
-      </c>
-      <c r="D3" t="n">
-        <v>20</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>https://lichess.org/mna6nw74</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>4041</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>blank</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>irBHYEJS</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>trashboatsr</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1890</v>
-      </c>
-      <c r="D4" t="n">
-        <v>100</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>https://lichess.org/irBHYEJS</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>4042</v>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>blank</t>
-        </is>
-      </c>
-    </row>
+    <row r="3" ht="18.75" customHeight="1"/>
+    <row r="4" ht="18.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added so many features - should be able to deploy?
</commit_message>
<xml_diff>
--- a/XL Spreadsheets/ChallengeMap.xlsx
+++ b/XL Spreadsheets/ChallengeMap.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,12 +28,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -64,18 +58,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -449,7 +440,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,23 +448,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-    <col width="27.29071428571428" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="7" max="7"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="8" max="8"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="27.29071428571428" bestFit="1" customWidth="1" style="4" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="8" max="8"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>gameID</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>challenger</t>
         </is>
@@ -488,7 +480,7 @@
           <t>wager</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>link</t>
         </is>
@@ -498,53 +490,63 @@
           <t>escrowID</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>accepted?</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>accepter</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>readyStatus</t>
+        </is>
+      </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1">
+    <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>bvarNUA0</t>
+          <t>xxjKVrHm</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>trashboatsr</t>
+          <t>RichDogeyBoy</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1890</v>
+        <v>1500</v>
       </c>
       <c r="D2" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://lichess.org/bvarNUA0</t>
+          <t>https://lichess.org/xxjKVrHm</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>4087</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
+        <v>4155</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>blank</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1"/>
-    <row r="4" ht="18.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>